<commit_message>
Added world map and line graph
</commit_message>
<xml_diff>
--- a/Data/Rejsevejledning.xlsx
+++ b/Data/Rejsevejledning.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$C$247</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$C$246</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,13 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="500">
-  <si>
-    <t>ABW</t>
-  </si>
-  <si>
-    <t>Aruba</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="500">
   <si>
     <t>AFG</t>
   </si>
@@ -1526,7 +1520,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>&lt;a href="https://um.dk/da/rejse-og-ophold/rejse-til-udlandet/rejsevejledninger/usa/"&gt;Klik her for rejsevejledning til USA&lt;/a&gt;</t>
+    <t>https://um.dk/da/rejse-og-ophold/rejse-til-udlandet/rejsevejledninger/usa/</t>
+  </si>
+  <si>
+    <t>Tekst</t>
+  </si>
+  <si>
+    <t>"Dette er en test"</t>
   </si>
 </sst>
 </file>
@@ -1860,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="D234" sqref="D234"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="E233" sqref="E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,21 +1872,24 @@
     <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C1" t="s">
-        <v>494</v>
-      </c>
       <c r="D1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1894,10 +1897,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1905,10 +1908,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1916,10 +1919,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1927,10 +1930,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1938,10 +1941,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1949,10 +1952,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1960,10 +1963,10 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1971,10 +1974,10 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1982,10 +1985,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1993,10 +1996,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2004,10 +2007,10 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2015,10 +2018,10 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2026,10 +2029,10 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -2037,10 +2040,10 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2059,7 +2062,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2070,7 +2073,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2084,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2095,7 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2106,7 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,7 +2117,7 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,7 +2128,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2139,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,7 +2161,7 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2172,7 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2183,7 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2194,7 @@
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,7 +2205,7 @@
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2216,7 @@
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2227,7 @@
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2238,7 @@
         <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,7 +2249,7 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,7 +2260,7 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2271,7 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2282,7 @@
         <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2293,7 @@
         <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2304,7 @@
         <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2315,7 @@
         <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2326,7 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2337,7 @@
         <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2348,7 @@
         <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2359,7 @@
         <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2370,7 @@
         <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,7 +2381,7 @@
         <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,7 +2392,7 @@
         <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2403,7 @@
         <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2414,7 @@
         <v>95</v>
       </c>
       <c r="C49" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2425,7 @@
         <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,7 +2436,7 @@
         <v>99</v>
       </c>
       <c r="C51" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2444,7 +2447,7 @@
         <v>101</v>
       </c>
       <c r="C52" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2455,7 +2458,7 @@
         <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,7 +2469,7 @@
         <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2480,7 @@
         <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2491,7 @@
         <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,7 +2502,7 @@
         <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,7 +2513,7 @@
         <v>113</v>
       </c>
       <c r="C58" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,7 +2524,7 @@
         <v>115</v>
       </c>
       <c r="C59" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,7 +2546,7 @@
         <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,7 +2557,7 @@
         <v>121</v>
       </c>
       <c r="C62" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,7 +2568,7 @@
         <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,7 +2579,7 @@
         <v>125</v>
       </c>
       <c r="C64" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,7 +2590,7 @@
         <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2598,7 +2601,7 @@
         <v>129</v>
       </c>
       <c r="C66" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2609,7 +2612,7 @@
         <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2620,7 +2623,7 @@
         <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2631,7 +2634,7 @@
         <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2642,7 +2645,7 @@
         <v>137</v>
       </c>
       <c r="C70" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2653,7 +2656,7 @@
         <v>139</v>
       </c>
       <c r="C71" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2664,7 +2667,7 @@
         <v>141</v>
       </c>
       <c r="C72" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2675,7 +2678,7 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,7 +2689,7 @@
         <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,7 +2700,7 @@
         <v>147</v>
       </c>
       <c r="C75" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2708,7 +2711,7 @@
         <v>149</v>
       </c>
       <c r="C76" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2719,7 +2722,7 @@
         <v>151</v>
       </c>
       <c r="C77" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2730,7 +2733,7 @@
         <v>153</v>
       </c>
       <c r="C78" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2741,7 +2744,7 @@
         <v>155</v>
       </c>
       <c r="C79" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,7 +2755,7 @@
         <v>157</v>
       </c>
       <c r="C80" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2763,7 +2766,7 @@
         <v>159</v>
       </c>
       <c r="C81" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2774,7 +2777,7 @@
         <v>161</v>
       </c>
       <c r="C82" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2785,7 +2788,7 @@
         <v>163</v>
       </c>
       <c r="C83" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2796,7 +2799,7 @@
         <v>165</v>
       </c>
       <c r="C84" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2807,7 +2810,7 @@
         <v>167</v>
       </c>
       <c r="C85" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2818,7 +2821,7 @@
         <v>169</v>
       </c>
       <c r="C86" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2832,7 @@
         <v>171</v>
       </c>
       <c r="C87" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,7 +2843,7 @@
         <v>173</v>
       </c>
       <c r="C88" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,7 +2854,7 @@
         <v>175</v>
       </c>
       <c r="C89" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2873,7 +2876,7 @@
         <v>179</v>
       </c>
       <c r="C91" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2884,7 +2887,7 @@
         <v>181</v>
       </c>
       <c r="C92" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2895,7 +2898,7 @@
         <v>183</v>
       </c>
       <c r="C93" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2906,7 +2909,7 @@
         <v>185</v>
       </c>
       <c r="C94" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2917,7 +2920,7 @@
         <v>187</v>
       </c>
       <c r="C95" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2928,7 +2931,7 @@
         <v>189</v>
       </c>
       <c r="C96" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2939,7 +2942,7 @@
         <v>191</v>
       </c>
       <c r="C97" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,7 +2953,7 @@
         <v>193</v>
       </c>
       <c r="C98" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2961,7 +2964,7 @@
         <v>195</v>
       </c>
       <c r="C99" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2972,7 +2975,7 @@
         <v>197</v>
       </c>
       <c r="C100" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2983,7 +2986,7 @@
         <v>199</v>
       </c>
       <c r="C101" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2994,7 +2997,7 @@
         <v>201</v>
       </c>
       <c r="C102" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3005,7 +3008,7 @@
         <v>203</v>
       </c>
       <c r="C103" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3016,7 +3019,7 @@
         <v>205</v>
       </c>
       <c r="C104" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3027,7 +3030,7 @@
         <v>207</v>
       </c>
       <c r="C105" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3038,7 +3041,7 @@
         <v>209</v>
       </c>
       <c r="C106" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3049,7 +3052,7 @@
         <v>211</v>
       </c>
       <c r="C107" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,7 +3063,7 @@
         <v>213</v>
       </c>
       <c r="C108" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3071,7 +3074,7 @@
         <v>215</v>
       </c>
       <c r="C109" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3082,7 +3085,7 @@
         <v>217</v>
       </c>
       <c r="C110" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3093,7 +3096,7 @@
         <v>219</v>
       </c>
       <c r="C111" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3115,7 +3118,7 @@
         <v>223</v>
       </c>
       <c r="C113" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3126,7 +3129,7 @@
         <v>225</v>
       </c>
       <c r="C114" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3137,7 +3140,7 @@
         <v>227</v>
       </c>
       <c r="C115" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,7 +3151,7 @@
         <v>229</v>
       </c>
       <c r="C116" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3159,7 +3162,7 @@
         <v>231</v>
       </c>
       <c r="C117" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3170,7 +3173,7 @@
         <v>233</v>
       </c>
       <c r="C118" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,7 +3184,7 @@
         <v>235</v>
       </c>
       <c r="C119" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3192,7 +3195,7 @@
         <v>237</v>
       </c>
       <c r="C120" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,7 +3206,7 @@
         <v>239</v>
       </c>
       <c r="C121" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3214,7 +3217,7 @@
         <v>241</v>
       </c>
       <c r="C122" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3225,7 +3228,7 @@
         <v>243</v>
       </c>
       <c r="C123" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3236,7 +3239,7 @@
         <v>245</v>
       </c>
       <c r="C124" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3247,7 +3250,7 @@
         <v>247</v>
       </c>
       <c r="C125" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3258,7 +3261,7 @@
         <v>249</v>
       </c>
       <c r="C126" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3269,7 +3272,7 @@
         <v>251</v>
       </c>
       <c r="C127" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3280,7 +3283,7 @@
         <v>253</v>
       </c>
       <c r="C128" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3291,7 +3294,7 @@
         <v>255</v>
       </c>
       <c r="C129" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,7 +3305,7 @@
         <v>257</v>
       </c>
       <c r="C130" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3313,7 +3316,7 @@
         <v>259</v>
       </c>
       <c r="C131" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -3324,7 +3327,7 @@
         <v>261</v>
       </c>
       <c r="C132" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -3335,7 +3338,7 @@
         <v>263</v>
       </c>
       <c r="C133" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3346,7 +3349,7 @@
         <v>265</v>
       </c>
       <c r="C134" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3357,7 +3360,7 @@
         <v>267</v>
       </c>
       <c r="C135" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3368,7 +3371,7 @@
         <v>269</v>
       </c>
       <c r="C136" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3379,7 +3382,7 @@
         <v>271</v>
       </c>
       <c r="C137" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -3390,7 +3393,7 @@
         <v>273</v>
       </c>
       <c r="C138" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,7 +3404,7 @@
         <v>275</v>
       </c>
       <c r="C139" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3412,7 +3415,7 @@
         <v>277</v>
       </c>
       <c r="C140" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -3423,7 +3426,7 @@
         <v>279</v>
       </c>
       <c r="C141" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -3434,7 +3437,7 @@
         <v>281</v>
       </c>
       <c r="C142" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -3445,7 +3448,7 @@
         <v>283</v>
       </c>
       <c r="C143" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,7 +3459,7 @@
         <v>285</v>
       </c>
       <c r="C144" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3470,7 @@
         <v>287</v>
       </c>
       <c r="C145" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3478,7 +3481,7 @@
         <v>289</v>
       </c>
       <c r="C146" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3489,7 +3492,7 @@
         <v>291</v>
       </c>
       <c r="C147" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3500,7 +3503,7 @@
         <v>293</v>
       </c>
       <c r="C148" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3511,7 +3514,7 @@
         <v>295</v>
       </c>
       <c r="C149" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3522,7 +3525,7 @@
         <v>297</v>
       </c>
       <c r="C150" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3533,7 +3536,7 @@
         <v>299</v>
       </c>
       <c r="C151" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3544,7 +3547,7 @@
         <v>301</v>
       </c>
       <c r="C152" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3555,7 +3558,7 @@
         <v>303</v>
       </c>
       <c r="C153" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3566,7 +3569,7 @@
         <v>305</v>
       </c>
       <c r="C154" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3577,7 +3580,7 @@
         <v>307</v>
       </c>
       <c r="C155" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3588,7 +3591,7 @@
         <v>309</v>
       </c>
       <c r="C156" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3599,7 +3602,7 @@
         <v>311</v>
       </c>
       <c r="C157" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3610,7 +3613,7 @@
         <v>313</v>
       </c>
       <c r="C158" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3621,7 +3624,7 @@
         <v>315</v>
       </c>
       <c r="C159" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3632,7 +3635,7 @@
         <v>317</v>
       </c>
       <c r="C160" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3643,7 +3646,7 @@
         <v>319</v>
       </c>
       <c r="C161" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,7 +3657,7 @@
         <v>321</v>
       </c>
       <c r="C162" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3665,7 +3668,7 @@
         <v>323</v>
       </c>
       <c r="C163" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3676,7 +3679,7 @@
         <v>325</v>
       </c>
       <c r="C164" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3687,7 +3690,7 @@
         <v>327</v>
       </c>
       <c r="C165" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3698,7 +3701,7 @@
         <v>329</v>
       </c>
       <c r="C166" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3709,7 +3712,7 @@
         <v>331</v>
       </c>
       <c r="C167" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3731,7 +3734,7 @@
         <v>335</v>
       </c>
       <c r="C169" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3742,7 +3745,7 @@
         <v>337</v>
       </c>
       <c r="C170" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,7 +3756,7 @@
         <v>339</v>
       </c>
       <c r="C171" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3764,7 +3767,7 @@
         <v>341</v>
       </c>
       <c r="C172" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3775,7 +3778,7 @@
         <v>343</v>
       </c>
       <c r="C173" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,7 +3789,7 @@
         <v>345</v>
       </c>
       <c r="C174" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3800,7 @@
         <v>347</v>
       </c>
       <c r="C175" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,7 +3811,7 @@
         <v>349</v>
       </c>
       <c r="C176" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3819,7 +3822,7 @@
         <v>351</v>
       </c>
       <c r="C177" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3830,7 +3833,7 @@
         <v>353</v>
       </c>
       <c r="C178" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3841,7 +3844,7 @@
         <v>355</v>
       </c>
       <c r="C179" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,7 +3866,7 @@
         <v>359</v>
       </c>
       <c r="C181" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,7 +3877,7 @@
         <v>361</v>
       </c>
       <c r="C182" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3888,7 @@
         <v>363</v>
       </c>
       <c r="C183" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,7 +3899,7 @@
         <v>365</v>
       </c>
       <c r="C184" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,7 +3910,7 @@
         <v>367</v>
       </c>
       <c r="C185" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -3918,7 +3921,7 @@
         <v>369</v>
       </c>
       <c r="C186" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -3929,7 +3932,7 @@
         <v>371</v>
       </c>
       <c r="C187" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -3940,7 +3943,7 @@
         <v>373</v>
       </c>
       <c r="C188" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3951,7 +3954,7 @@
         <v>375</v>
       </c>
       <c r="C189" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3962,7 +3965,7 @@
         <v>377</v>
       </c>
       <c r="C190" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -3973,7 +3976,7 @@
         <v>379</v>
       </c>
       <c r="C191" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -3984,7 +3987,7 @@
         <v>381</v>
       </c>
       <c r="C192" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -3995,7 +3998,7 @@
         <v>383</v>
       </c>
       <c r="C193" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -4006,7 +4009,7 @@
         <v>385</v>
       </c>
       <c r="C194" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4017,7 +4020,7 @@
         <v>387</v>
       </c>
       <c r="C195" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4028,7 +4031,7 @@
         <v>389</v>
       </c>
       <c r="C196" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -4039,7 +4042,7 @@
         <v>391</v>
       </c>
       <c r="C197" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4050,7 +4053,7 @@
         <v>393</v>
       </c>
       <c r="C198" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4061,7 +4064,7 @@
         <v>395</v>
       </c>
       <c r="C199" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4072,7 +4075,7 @@
         <v>397</v>
       </c>
       <c r="C200" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4083,7 +4086,7 @@
         <v>399</v>
       </c>
       <c r="C201" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4094,7 +4097,7 @@
         <v>401</v>
       </c>
       <c r="C202" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4105,7 +4108,7 @@
         <v>403</v>
       </c>
       <c r="C203" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4116,7 +4119,7 @@
         <v>405</v>
       </c>
       <c r="C204" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4127,7 +4130,7 @@
         <v>407</v>
       </c>
       <c r="C205" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4138,7 +4141,7 @@
         <v>409</v>
       </c>
       <c r="C206" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4149,7 +4152,7 @@
         <v>411</v>
       </c>
       <c r="C207" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -4160,7 +4163,7 @@
         <v>413</v>
       </c>
       <c r="C208" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4171,7 +4174,7 @@
         <v>415</v>
       </c>
       <c r="C209" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4182,7 +4185,7 @@
         <v>417</v>
       </c>
       <c r="C210" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4193,7 +4196,7 @@
         <v>419</v>
       </c>
       <c r="C211" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -4204,7 +4207,7 @@
         <v>421</v>
       </c>
       <c r="C212" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -4215,7 +4218,7 @@
         <v>423</v>
       </c>
       <c r="C213" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -4226,7 +4229,7 @@
         <v>425</v>
       </c>
       <c r="C214" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4237,7 +4240,7 @@
         <v>427</v>
       </c>
       <c r="C215" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -4248,7 +4251,7 @@
         <v>429</v>
       </c>
       <c r="C216" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4259,7 +4262,7 @@
         <v>431</v>
       </c>
       <c r="C217" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4270,7 +4273,7 @@
         <v>433</v>
       </c>
       <c r="C218" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4281,7 +4284,7 @@
         <v>435</v>
       </c>
       <c r="C219" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -4292,7 +4295,7 @@
         <v>437</v>
       </c>
       <c r="C220" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -4303,7 +4306,7 @@
         <v>439</v>
       </c>
       <c r="C221" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4314,7 +4317,7 @@
         <v>441</v>
       </c>
       <c r="C222" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -4325,7 +4328,7 @@
         <v>443</v>
       </c>
       <c r="C223" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -4336,10 +4339,10 @@
         <v>445</v>
       </c>
       <c r="C224" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>446</v>
       </c>
@@ -4347,10 +4350,10 @@
         <v>447</v>
       </c>
       <c r="C225" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>448</v>
       </c>
@@ -4358,10 +4361,10 @@
         <v>449</v>
       </c>
       <c r="C226" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>450</v>
       </c>
@@ -4369,10 +4372,10 @@
         <v>451</v>
       </c>
       <c r="C227" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>452</v>
       </c>
@@ -4380,10 +4383,10 @@
         <v>453</v>
       </c>
       <c r="C228" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>454</v>
       </c>
@@ -4391,10 +4394,10 @@
         <v>455</v>
       </c>
       <c r="C229" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>456</v>
       </c>
@@ -4402,10 +4405,10 @@
         <v>457</v>
       </c>
       <c r="C230" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>458</v>
       </c>
@@ -4413,10 +4416,11 @@
         <v>459</v>
       </c>
       <c r="C231" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+      <c r="D231" s="2"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>460</v>
       </c>
@@ -4424,11 +4428,16 @@
         <v>461</v>
       </c>
       <c r="C232" t="s">
+        <v>495</v>
+      </c>
+      <c r="D232" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D232" s="2"/>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>462</v>
       </c>
@@ -4436,13 +4445,10 @@
         <v>463</v>
       </c>
       <c r="C233" t="s">
-        <v>497</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>464</v>
       </c>
@@ -4450,10 +4456,10 @@
         <v>465</v>
       </c>
       <c r="C234" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>466</v>
       </c>
@@ -4461,10 +4467,10 @@
         <v>467</v>
       </c>
       <c r="C235" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>468</v>
       </c>
@@ -4472,10 +4478,10 @@
         <v>469</v>
       </c>
       <c r="C236" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>470</v>
       </c>
@@ -4483,10 +4489,10 @@
         <v>471</v>
       </c>
       <c r="C237" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>472</v>
       </c>
@@ -4494,10 +4500,10 @@
         <v>473</v>
       </c>
       <c r="C238" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>474</v>
       </c>
@@ -4505,10 +4511,10 @@
         <v>475</v>
       </c>
       <c r="C239" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>476</v>
       </c>
@@ -4516,7 +4522,7 @@
         <v>477</v>
       </c>
       <c r="C240" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4527,7 +4533,7 @@
         <v>479</v>
       </c>
       <c r="C241" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4538,7 +4544,7 @@
         <v>481</v>
       </c>
       <c r="C242" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4549,7 +4555,7 @@
         <v>483</v>
       </c>
       <c r="C243" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4560,7 +4566,7 @@
         <v>485</v>
       </c>
       <c r="C244" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4571,7 +4577,7 @@
         <v>487</v>
       </c>
       <c r="C245" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,22 +4588,11 @@
         <v>489</v>
       </c>
       <c r="C246" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B247" t="s">
-        <v>491</v>
-      </c>
-      <c r="C247" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C247"/>
+  <autoFilter ref="A1:C246"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>